<commit_message>
Modified Test Scripts for Merchant Portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testdata-merchant.xlsx
+++ b/Web/coyni/resources/testdata-merchant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Merchant - Sanity Testing\clone_Merchant_sanity_27_12_2022\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F18FAF7-9040-4E9F-A833-494E470412E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC107C2-57A3-476E-9E91-0CACE66DB398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16020" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="withdrawToUSDCogent" sheetId="37" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="659">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2009,6 +2009,15 @@
   </si>
   <si>
     <t>2-Step Authentication</t>
+  </si>
+  <si>
+    <t>transactionHeading</t>
+  </si>
+  <si>
+    <t>payOutHistoryHeading</t>
+  </si>
+  <si>
+    <t>reserveHistoryHeading</t>
   </si>
 </sst>
 </file>
@@ -2586,33 +2595,33 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" customWidth="1"/>
-    <col min="10" max="10" width="22.109375" customWidth="1"/>
-    <col min="11" max="12" width="24.6640625" customWidth="1"/>
-    <col min="15" max="15" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="12" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1"/>
     <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="17.5546875" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1"/>
-    <col min="24" max="24" width="19.5546875" customWidth="1"/>
-    <col min="25" max="25" width="24.5546875" customWidth="1"/>
-    <col min="26" max="26" width="15.109375" customWidth="1"/>
-    <col min="27" max="27" width="16.109375" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" customWidth="1"/>
+    <col min="25" max="25" width="24.5703125" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>357</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>358</v>
       </c>
@@ -2845,7 +2854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>358</v>
       </c>
@@ -2899,7 +2908,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>358</v>
       </c>
@@ -2953,7 +2962,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>359</v>
       </c>
@@ -3027,28 +3036,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B794F90B-B775-49C2-A1ED-1F487FA3454C}">
-  <dimension ref="A1:AB41"/>
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="18" width="20.44140625" customWidth="1"/>
-    <col min="19" max="20" width="19.88671875" customWidth="1"/>
-    <col min="21" max="28" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="21" width="20.42578125" customWidth="1"/>
+    <col min="22" max="23" width="19.85546875" customWidth="1"/>
+    <col min="24" max="31" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3089,52 +3098,61 @@
         <v>420</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>423</v>
       </c>
@@ -3169,7 +3187,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>426</v>
       </c>
@@ -3204,7 +3222,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>428</v>
       </c>
@@ -3239,7 +3257,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>430</v>
       </c>
@@ -3274,7 +3292,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -3305,29 +3323,29 @@
       <c r="J6" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="W6" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
         <v>219</v>
       </c>
-      <c r="V6" t="s">
+      <c r="Y6" t="s">
         <v>116</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>25</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AE6" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -3368,8 +3386,11 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3410,8 +3431,11 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3452,8 +3476,11 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -3494,8 +3521,11 @@
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -3536,8 +3566,11 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -3573,21 +3606,24 @@
         <v>433</v>
       </c>
       <c r="M12" s="8"/>
-      <c r="N12" s="24">
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="24">
         <v>1</v>
       </c>
-      <c r="O12" s="24">
+      <c r="R12" s="24">
         <v>10</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="S12" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="T12" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="R12" s="24"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U12" s="24"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -3623,21 +3659,24 @@
         <v>436</v>
       </c>
       <c r="M13" s="8"/>
-      <c r="N13" s="24">
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="24">
         <v>1</v>
       </c>
-      <c r="O13" s="24">
+      <c r="R13" s="24">
         <v>10</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="S13" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="T13" s="24" t="s">
         <v>436</v>
       </c>
-      <c r="R13" s="24"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U13" s="24"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>234</v>
       </c>
@@ -3673,21 +3712,24 @@
         <v>239</v>
       </c>
       <c r="M14" s="8"/>
-      <c r="N14" s="24">
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="24">
         <v>1</v>
       </c>
-      <c r="O14" s="24">
+      <c r="R14" s="24">
         <v>10</v>
       </c>
-      <c r="P14" s="24" t="s">
+      <c r="S14" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q14" s="24" t="s">
+      <c r="T14" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="R14" s="24"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U14" s="24"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -3723,21 +3765,24 @@
         <v>440</v>
       </c>
       <c r="M15" s="8"/>
-      <c r="N15" s="24">
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="24">
         <v>1</v>
       </c>
-      <c r="O15" s="24">
+      <c r="R15" s="24">
         <v>10</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="S15" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="T15" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="R15" s="24"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U15" s="24"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>249</v>
       </c>
@@ -3773,21 +3818,24 @@
         <v>433</v>
       </c>
       <c r="M16" s="8"/>
-      <c r="N16" s="24">
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="24">
         <v>1</v>
       </c>
-      <c r="O16" s="24">
+      <c r="R16" s="24">
         <v>10</v>
       </c>
-      <c r="P16" s="24" t="s">
+      <c r="S16" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q16" s="24" t="s">
+      <c r="T16" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="R16" s="24"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U16" s="24"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>249</v>
       </c>
@@ -3823,21 +3871,24 @@
         <v>436</v>
       </c>
       <c r="M17" s="8"/>
-      <c r="N17" s="24">
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="24">
         <v>1</v>
       </c>
-      <c r="O17" s="24">
+      <c r="R17" s="24">
         <v>10</v>
       </c>
-      <c r="P17" s="24" t="s">
+      <c r="S17" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q17" s="24" t="s">
+      <c r="T17" s="24" t="s">
         <v>436</v>
       </c>
-      <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U17" s="24"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>249</v>
       </c>
@@ -3873,21 +3924,24 @@
         <v>239</v>
       </c>
       <c r="M18" s="8"/>
-      <c r="N18" s="24">
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="24">
         <v>1</v>
       </c>
-      <c r="O18" s="24">
+      <c r="R18" s="24">
         <v>10</v>
       </c>
-      <c r="P18" s="24" t="s">
+      <c r="S18" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q18" s="24" t="s">
+      <c r="T18" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="U18" s="24"/>
+    </row>
+    <row r="19" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>249</v>
       </c>
@@ -3923,21 +3977,24 @@
         <v>440</v>
       </c>
       <c r="M19" s="8"/>
-      <c r="N19" s="24">
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="24">
         <v>1</v>
       </c>
-      <c r="O19" s="24">
+      <c r="R19" s="24">
         <v>10</v>
       </c>
-      <c r="P19" s="24" t="s">
+      <c r="S19" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="Q19" s="24" t="s">
+      <c r="T19" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="U19" s="24"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>444</v>
       </c>
@@ -3978,8 +4035,11 @@
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>447</v>
       </c>
@@ -4020,8 +4080,11 @@
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>450</v>
       </c>
@@ -4062,8 +4125,11 @@
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>452</v>
       </c>
@@ -4104,8 +4170,11 @@
       <c r="P23" s="24"/>
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>454</v>
       </c>
@@ -4145,11 +4214,14 @@
       <c r="O24" s="24"/>
       <c r="P24" s="24"/>
       <c r="Q24" s="24"/>
-      <c r="R24" s="24" t="s">
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>457</v>
       </c>
@@ -4184,7 +4256,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>459</v>
       </c>
@@ -4224,8 +4296,11 @@
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
       <c r="Q26" s="24"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>461</v>
       </c>
@@ -4265,8 +4340,11 @@
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
       <c r="Q27" s="24"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>463</v>
       </c>
@@ -4306,8 +4384,11 @@
       <c r="O28" s="24"/>
       <c r="P28" s="24"/>
       <c r="Q28" s="24"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>465</v>
       </c>
@@ -4347,8 +4428,11 @@
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>467</v>
       </c>
@@ -4388,8 +4472,11 @@
       <c r="O30" s="24"/>
       <c r="P30" s="24"/>
       <c r="Q30" s="24"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>469</v>
       </c>
@@ -4429,11 +4516,14 @@
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
       <c r="Q31" s="24"/>
-      <c r="R31" t="s">
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>472</v>
       </c>
@@ -4473,8 +4563,11 @@
       <c r="O32" s="24"/>
       <c r="P32" s="24"/>
       <c r="Q32" s="24"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>474</v>
       </c>
@@ -4514,8 +4607,11 @@
       <c r="O33" s="24"/>
       <c r="P33" s="24"/>
       <c r="Q33" s="24"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>476</v>
       </c>
@@ -4553,8 +4649,11 @@
         <v>239</v>
       </c>
       <c r="M34" s="8"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>479</v>
       </c>
@@ -4592,7 +4691,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>481</v>
       </c>
@@ -4630,7 +4729,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>483</v>
       </c>
@@ -4668,7 +4767,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>485</v>
       </c>
@@ -4703,7 +4802,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>487</v>
       </c>
@@ -4744,7 +4843,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>489</v>
       </c>
@@ -4785,7 +4884,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>490</v>
       </c>
@@ -4818,6 +4917,15 @@
       </c>
       <c r="K41" t="s">
         <v>425</v>
+      </c>
+      <c r="N41" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="O41" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="P41" s="19" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -4889,6 +4997,7 @@
     <hyperlink ref="E41" r:id="rId65" xr:uid="{FE6F8951-114D-4293-A9CE-C709981D9AF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 
@@ -4900,35 +5009,35 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="77.88671875" customWidth="1"/>
-    <col min="5" max="5" width="35.88671875" customWidth="1"/>
-    <col min="6" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="10" width="35.88671875" customWidth="1"/>
-    <col min="11" max="11" width="35.109375" customWidth="1"/>
-    <col min="12" max="13" width="13.44140625" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="15" max="15" width="49.109375" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="6" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="10" width="35.85546875" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="12" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="49.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.88671875" customWidth="1"/>
-    <col min="22" max="22" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="19.109375" customWidth="1"/>
-    <col min="26" max="26" width="29.109375" customWidth="1"/>
-    <col min="27" max="27" width="19.109375" customWidth="1"/>
-    <col min="28" max="28" width="21.6640625" customWidth="1"/>
-    <col min="29" max="29" width="24.33203125" customWidth="1"/>
-    <col min="30" max="30" width="23.88671875" customWidth="1"/>
-    <col min="31" max="31" width="11.44140625"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.85546875" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="19.140625" customWidth="1"/>
+    <col min="26" max="26" width="29.140625" customWidth="1"/>
+    <col min="27" max="27" width="19.140625" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" customWidth="1"/>
+    <col min="29" max="29" width="24.28515625" customWidth="1"/>
+    <col min="30" max="30" width="23.85546875" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -5023,7 +5132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>149</v>
       </c>
@@ -5064,7 +5173,7 @@
       <c r="Z2" s="10"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>207</v>
       </c>
@@ -5134,7 +5243,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="134.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>206</v>
       </c>
@@ -5175,7 +5284,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>205</v>
       </c>
@@ -5225,7 +5334,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>205</v>
       </c>
@@ -5273,7 +5382,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>205</v>
       </c>
@@ -5322,7 +5431,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>205</v>
       </c>
@@ -5371,7 +5480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>205</v>
       </c>
@@ -5420,7 +5529,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>205</v>
       </c>
@@ -5471,7 +5580,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>205</v>
       </c>
@@ -5517,7 +5626,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>205</v>
       </c>
@@ -5565,7 +5674,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>205</v>
       </c>
@@ -5613,7 +5722,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>205</v>
       </c>
@@ -5661,7 +5770,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>205</v>
       </c>
@@ -5709,7 +5818,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>205</v>
       </c>
@@ -5757,7 +5866,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>205</v>
       </c>
@@ -5805,7 +5914,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>205</v>
       </c>
@@ -5853,7 +5962,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>205</v>
       </c>
@@ -5899,7 +6008,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>205</v>
       </c>
@@ -5945,7 +6054,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>205</v>
       </c>
@@ -5993,7 +6102,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>274</v>
       </c>
@@ -6026,7 +6135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>289</v>
       </c>
@@ -6062,7 +6171,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>292</v>
       </c>
@@ -6098,7 +6207,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>294</v>
       </c>
@@ -6134,7 +6243,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>296</v>
       </c>
@@ -6170,7 +6279,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>298</v>
       </c>
@@ -6203,7 +6312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>205</v>
       </c>
@@ -6221,7 +6330,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>319</v>
       </c>
@@ -6278,7 +6387,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>327</v>
       </c>
@@ -6296,7 +6405,7 @@
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>329</v>
       </c>
@@ -6347,7 +6456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>347</v>
       </c>
@@ -6474,45 +6583,45 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" customWidth="1"/>
-    <col min="9" max="9" width="31.44140625" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="34" customWidth="1"/>
-    <col min="14" max="14" width="27.5546875" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" customWidth="1"/>
-    <col min="18" max="18" width="29.44140625" customWidth="1"/>
-    <col min="19" max="19" width="24.6640625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="29.42578125" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" customWidth="1"/>
     <col min="20" max="20" width="41" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.109375" customWidth="1"/>
-    <col min="24" max="24" width="22.6640625" customWidth="1"/>
-    <col min="25" max="25" width="16.44140625" customWidth="1"/>
-    <col min="26" max="26" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="19.44140625" customWidth="1"/>
-    <col min="28" max="29" width="20.44140625" customWidth="1"/>
-    <col min="30" max="30" width="17.5546875" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="26" max="26" width="19.28515625" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" customWidth="1"/>
+    <col min="28" max="29" width="20.42578125" customWidth="1"/>
+    <col min="30" max="30" width="17.5703125" customWidth="1"/>
     <col min="31" max="31" width="20" customWidth="1"/>
     <col min="32" max="32" width="16" customWidth="1"/>
-    <col min="33" max="33" width="30.6640625" customWidth="1"/>
+    <col min="33" max="33" width="30.7109375" customWidth="1"/>
     <col min="34" max="34" width="14" customWidth="1"/>
     <col min="35" max="35" width="13" customWidth="1"/>
-    <col min="36" max="36" width="15.6640625" customWidth="1"/>
-    <col min="37" max="37" width="16.88671875" customWidth="1"/>
-    <col min="38" max="38" width="33.33203125" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" customWidth="1"/>
+    <col min="38" max="38" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6628,7 +6737,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>550</v>
       </c>
@@ -6696,7 +6805,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>557</v>
       </c>
@@ -6758,7 +6867,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>557</v>
       </c>
@@ -6817,7 +6926,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>557</v>
       </c>
@@ -6876,7 +6985,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>562</v>
       </c>
@@ -6935,7 +7044,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>564</v>
       </c>
@@ -7009,7 +7118,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>573</v>
       </c>
@@ -7083,7 +7192,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>579</v>
       </c>
@@ -7127,7 +7236,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="250.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>582</v>
       </c>
@@ -7196,7 +7305,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>582</v>
       </c>
@@ -7252,7 +7361,7 @@
       <c r="AJ11" s="20"/>
       <c r="AK11" s="20"/>
     </row>
-    <row r="12" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>582</v>
       </c>
@@ -7311,7 +7420,7 @@
       <c r="AJ12" s="20"/>
       <c r="AK12" s="20"/>
     </row>
-    <row r="13" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>582</v>
       </c>
@@ -7376,7 +7485,7 @@
       <c r="AJ13" s="20"/>
       <c r="AK13" s="20"/>
     </row>
-    <row r="14" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>582</v>
       </c>
@@ -7432,7 +7541,7 @@
       <c r="AJ14" s="20"/>
       <c r="AK14" s="20"/>
     </row>
-    <row r="15" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>582</v>
       </c>
@@ -7491,7 +7600,7 @@
       <c r="AJ15" s="20"/>
       <c r="AK15" s="20"/>
     </row>
-    <row r="16" spans="1:38" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>582</v>
       </c>
@@ -7559,7 +7668,7 @@
       <c r="AJ16" s="20"/>
       <c r="AK16" s="20"/>
     </row>
-    <row r="17" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>582</v>
       </c>
@@ -7634,7 +7743,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>582</v>
       </c>
@@ -7709,7 +7818,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>619</v>
       </c>
@@ -7768,7 +7877,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>619</v>
       </c>
@@ -7827,7 +7936,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>619</v>
       </c>
@@ -7886,7 +7995,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>619</v>
       </c>
@@ -7945,7 +8054,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>621</v>
       </c>
@@ -8028,7 +8137,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>621</v>
       </c>
@@ -8111,7 +8220,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>621</v>
       </c>
@@ -8194,7 +8303,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>621</v>
       </c>
@@ -8274,7 +8383,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>621</v>
       </c>
@@ -8354,7 +8463,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>621</v>
       </c>
@@ -8434,7 +8543,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>621</v>
       </c>
@@ -8514,7 +8623,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>621</v>
       </c>
@@ -8594,7 +8703,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>621</v>
       </c>
@@ -8674,7 +8783,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>621</v>
       </c>
@@ -8754,7 +8863,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>621</v>
       </c>
@@ -8834,7 +8943,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>621</v>
       </c>
@@ -8914,7 +9023,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>621</v>
       </c>
@@ -9018,28 +9127,28 @@
       <selection pane="topRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="9" width="63.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="9" width="63.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="14" width="33.88671875" customWidth="1"/>
-    <col min="15" max="15" width="24.44140625" customWidth="1"/>
-    <col min="16" max="16" width="26.44140625" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="19.88671875" customWidth="1"/>
-    <col min="19" max="19" width="17.44140625" customWidth="1"/>
-    <col min="20" max="20" width="31.88671875" customWidth="1"/>
-    <col min="23" max="23" width="19.88671875" customWidth="1"/>
+    <col min="12" max="14" width="33.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="31.85546875" customWidth="1"/>
+    <col min="23" max="23" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9119,7 +9228,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>209</v>
       </c>
@@ -9157,7 +9266,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>364</v>
       </c>
@@ -9193,7 +9302,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -9226,7 +9335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -9259,7 +9368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>210</v>
       </c>
@@ -9294,7 +9403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>210</v>
       </c>
@@ -9329,7 +9438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -9367,7 +9476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9391,7 +9500,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -9429,7 +9538,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>211</v>
       </c>
@@ -9461,7 +9570,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -9493,7 +9602,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -9525,7 +9634,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -9557,7 +9666,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -9586,7 +9695,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -9620,7 +9729,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -9652,7 +9761,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -9681,7 +9790,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -9710,7 +9819,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -9739,7 +9848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -9771,7 +9880,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -9803,7 +9912,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>325</v>
       </c>
@@ -9838,7 +9947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>333</v>
       </c>
@@ -9873,7 +9982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>492</v>
       </c>
@@ -9960,40 +10069,40 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="20.5546875" customWidth="1"/>
-    <col min="15" max="15" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.5546875" customWidth="1"/>
-    <col min="21" max="21" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="20.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.44140625" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.42578125" customWidth="1"/>
     <col min="27" max="27" width="34" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="42" customWidth="1"/>
-    <col min="29" max="29" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="70.88671875" customWidth="1"/>
-    <col min="32" max="32" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="70.85546875" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10091,7 +10200,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>395</v>
       </c>
@@ -10177,27 +10286,27 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="32.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1"/>
-    <col min="12" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="18" width="17.44140625" customWidth="1"/>
-    <col min="19" max="19" width="15.88671875" customWidth="1"/>
-    <col min="20" max="20" width="20.44140625" customWidth="1"/>
-    <col min="21" max="21" width="32.44140625" customWidth="1"/>
+    <col min="16" max="18" width="17.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" customWidth="1"/>
+    <col min="21" max="21" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10262,7 +10371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>532</v>
       </c>
@@ -10324,7 +10433,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>541</v>
       </c>
@@ -10375,45 +10484,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD80F779-3731-469C-B080-C0C15FEDCBB1}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="31" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" customWidth="1"/>
-    <col min="13" max="16" width="25.5546875" customWidth="1"/>
-    <col min="17" max="17" width="31.77734375" customWidth="1"/>
-    <col min="18" max="23" width="25.5546875" customWidth="1"/>
-    <col min="24" max="24" width="22.6640625" customWidth="1"/>
-    <col min="25" max="25" width="14.88671875" customWidth="1"/>
-    <col min="26" max="26" width="17.5546875" customWidth="1"/>
-    <col min="28" max="28" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" customWidth="1"/>
+    <col min="18" max="23" width="25.5703125" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" customWidth="1"/>
+    <col min="26" max="26" width="17.5703125" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" customWidth="1"/>
     <col min="29" max="29" width="12" customWidth="1"/>
-    <col min="30" max="30" width="26.88671875" customWidth="1"/>
-    <col min="32" max="32" width="23.5546875" customWidth="1"/>
-    <col min="33" max="33" width="23.33203125" customWidth="1"/>
-    <col min="35" max="35" width="31.5546875" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" customWidth="1"/>
-    <col min="37" max="37" width="28.44140625" customWidth="1"/>
+    <col min="30" max="30" width="26.85546875" customWidth="1"/>
+    <col min="32" max="32" width="23.5703125" customWidth="1"/>
+    <col min="33" max="33" width="23.28515625" customWidth="1"/>
+    <col min="35" max="35" width="31.5703125" customWidth="1"/>
+    <col min="36" max="36" width="19.7109375" customWidth="1"/>
+    <col min="37" max="37" width="28.42578125" customWidth="1"/>
     <col min="38" max="38" width="33" customWidth="1"/>
-    <col min="39" max="39" width="35.44140625" customWidth="1"/>
-    <col min="40" max="40" width="31.33203125" customWidth="1"/>
-    <col min="41" max="41" width="43.6640625" customWidth="1"/>
-    <col min="42" max="42" width="36.109375" customWidth="1"/>
-    <col min="43" max="43" width="43.88671875" customWidth="1"/>
+    <col min="39" max="39" width="35.42578125" customWidth="1"/>
+    <col min="40" max="40" width="31.28515625" customWidth="1"/>
+    <col min="41" max="41" width="43.7109375" customWidth="1"/>
+    <col min="42" max="42" width="36.140625" customWidth="1"/>
+    <col min="43" max="43" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10541,7 +10650,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>418</v>
       </c>
@@ -10608,52 +10717,52 @@
       <selection activeCell="BO3" sqref="BO3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
-    <col min="12" max="16" width="20.44140625" customWidth="1"/>
-    <col min="17" max="17" width="19.88671875" customWidth="1"/>
-    <col min="18" max="18" width="19.88671875" hidden="1" customWidth="1"/>
-    <col min="19" max="21" width="19.88671875" customWidth="1"/>
-    <col min="22" max="26" width="30.109375" customWidth="1"/>
-    <col min="27" max="38" width="28.44140625" customWidth="1"/>
-    <col min="39" max="39" width="19.88671875" customWidth="1"/>
-    <col min="40" max="40" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="12" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="21" width="19.85546875" customWidth="1"/>
+    <col min="22" max="26" width="30.140625" customWidth="1"/>
+    <col min="27" max="38" width="28.42578125" customWidth="1"/>
+    <col min="39" max="39" width="19.85546875" customWidth="1"/>
+    <col min="40" max="40" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="45" width="23" customWidth="1"/>
-    <col min="46" max="46" width="26.109375" customWidth="1"/>
+    <col min="46" max="46" width="26.140625" customWidth="1"/>
     <col min="47" max="47" width="28" customWidth="1"/>
-    <col min="48" max="48" width="18.109375" customWidth="1"/>
+    <col min="48" max="48" width="18.140625" customWidth="1"/>
     <col min="49" max="49" width="17" customWidth="1"/>
-    <col min="50" max="50" width="17.44140625" customWidth="1"/>
+    <col min="50" max="50" width="17.42578125" customWidth="1"/>
     <col min="51" max="51" width="15" customWidth="1"/>
-    <col min="52" max="52" width="22.44140625" customWidth="1"/>
-    <col min="53" max="53" width="20.109375" customWidth="1"/>
-    <col min="54" max="54" width="12.88671875" customWidth="1"/>
-    <col min="55" max="55" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.6640625" customWidth="1"/>
-    <col min="61" max="61" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.42578125" customWidth="1"/>
+    <col min="53" max="53" width="20.140625" customWidth="1"/>
+    <col min="54" max="54" width="12.85546875" customWidth="1"/>
+    <col min="55" max="55" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.7109375" customWidth="1"/>
+    <col min="61" max="61" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10853,7 +10962,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -10885,7 +10994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>286</v>
       </c>
@@ -10927,7 +11036,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>251</v>
       </c>
@@ -10969,7 +11078,7 @@
       </c>
       <c r="P4" s="19"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>253</v>
       </c>
@@ -11011,7 +11120,7 @@
       </c>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -11052,7 +11161,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>257</v>
       </c>
@@ -11093,7 +11202,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>259</v>
       </c>
@@ -11135,7 +11244,7 @@
       </c>
       <c r="P8" s="8"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>261</v>
       </c>
@@ -11176,7 +11285,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>263</v>
       </c>
@@ -11220,7 +11329,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -11264,7 +11373,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>265</v>
       </c>
@@ -11299,7 +11408,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>267</v>
       </c>
@@ -11337,7 +11446,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>269</v>
       </c>
@@ -11407,43 +11516,43 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" customWidth="1"/>
-    <col min="13" max="13" width="19.88671875" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="19.88671875" customWidth="1"/>
-    <col min="18" max="22" width="30.109375" customWidth="1"/>
-    <col min="23" max="30" width="28.44140625" customWidth="1"/>
-    <col min="31" max="33" width="22.109375" customWidth="1"/>
-    <col min="34" max="38" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="19.85546875" customWidth="1"/>
+    <col min="18" max="22" width="30.140625" customWidth="1"/>
+    <col min="23" max="30" width="28.42578125" customWidth="1"/>
+    <col min="31" max="33" width="22.140625" customWidth="1"/>
+    <col min="34" max="38" width="19.85546875" customWidth="1"/>
     <col min="39" max="39" width="50" customWidth="1"/>
-    <col min="40" max="40" width="22.44140625" customWidth="1"/>
-    <col min="41" max="41" width="16.109375" customWidth="1"/>
+    <col min="40" max="40" width="22.42578125" customWidth="1"/>
+    <col min="41" max="41" width="16.140625" customWidth="1"/>
     <col min="44" max="44" width="22" customWidth="1"/>
-    <col min="45" max="45" width="21.44140625" customWidth="1"/>
-    <col min="47" max="47" width="17.88671875" customWidth="1"/>
+    <col min="45" max="45" width="21.42578125" customWidth="1"/>
+    <col min="47" max="47" width="17.85546875" customWidth="1"/>
     <col min="48" max="48" width="23" customWidth="1"/>
-    <col min="49" max="49" width="16.44140625" customWidth="1"/>
-    <col min="50" max="50" width="26.109375" customWidth="1"/>
+    <col min="49" max="49" width="16.42578125" customWidth="1"/>
+    <col min="50" max="50" width="26.140625" customWidth="1"/>
     <col min="51" max="52" width="28" customWidth="1"/>
-    <col min="53" max="53" width="18.109375" customWidth="1"/>
+    <col min="53" max="53" width="18.140625" customWidth="1"/>
     <col min="54" max="54" width="17" customWidth="1"/>
-    <col min="55" max="55" width="17.44140625" customWidth="1"/>
+    <col min="55" max="55" width="17.42578125" customWidth="1"/>
     <col min="56" max="56" width="15" customWidth="1"/>
-    <col min="57" max="57" width="22.44140625" customWidth="1"/>
-    <col min="58" max="58" width="20.109375" customWidth="1"/>
-    <col min="59" max="59" width="12.88671875" customWidth="1"/>
+    <col min="57" max="57" width="22.42578125" customWidth="1"/>
+    <col min="58" max="58" width="20.140625" customWidth="1"/>
+    <col min="59" max="59" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11628,7 +11737,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>519</v>
       </c>
@@ -11663,7 +11772,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>521</v>
       </c>
@@ -11698,7 +11807,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>523</v>
       </c>

</xml_diff>